<commit_message>
dectypted by 2 bijections
</commit_message>
<xml_diff>
--- a/lab_1/task2/tables.xlsx
+++ b/lab_1/task2/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\working\inform-security-base\inform-security-base\lab_1\task2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniversityLabs\inform-security-base\lab_1\task2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C994CB9B-C558-4859-BAE5-52E9A1B4224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3DDE98-291D-4793-A940-F8CB08033059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="89">
   <si>
     <t>Результат анализа</t>
   </si>
@@ -223,6 +223,78 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S </t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -247,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,12 +328,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,11 +347,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -283,7 +376,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -564,21 +659,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -588,7 +683,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -602,7 +697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -618,11 +713,14 @@
       <c r="I3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -635,14 +733,17 @@
       <c r="F4" s="2">
         <v>9.3637454981992801E-2</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -655,14 +756,17 @@
       <c r="F5" s="2">
         <v>9.1236494597839099E-2</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -675,14 +779,17 @@
       <c r="F6" s="2">
         <v>7.8031212484993895E-2</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,14 +802,17 @@
       <c r="F7" s="2">
         <v>6.4825930372148802E-2</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -715,14 +825,17 @@
       <c r="F8" s="2">
         <v>6.1224489795918297E-2</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -735,14 +848,17 @@
       <c r="F9" s="2">
         <v>5.6422569027611003E-2</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -755,14 +871,17 @@
       <c r="F10" s="2">
         <v>5.52220888355342E-2</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="7">
         <v>9</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -775,14 +894,17 @@
       <c r="F11" s="2">
         <v>4.2016806722689003E-2</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -795,14 +917,17 @@
       <c r="F12" s="2">
         <v>3.6014405762304899E-2</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -815,14 +940,17 @@
       <c r="F13" s="2">
         <v>2.76110444177671E-2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="7">
         <v>1</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -835,14 +963,17 @@
       <c r="F14" s="2">
         <v>2.76110444177671E-2</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -855,14 +986,17 @@
       <c r="F15" s="2">
         <v>2.4009603841536602E-2</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="7">
         <v>3</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -875,14 +1009,17 @@
       <c r="F16" s="2">
         <v>2.1608643457382899E-2</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -895,14 +1032,17 @@
       <c r="F17" s="2">
         <v>1.92076830732292E-2</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -915,14 +1055,17 @@
       <c r="F18" s="2">
         <v>1.8007202881152401E-2</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -935,14 +1078,17 @@
       <c r="F19" s="2">
         <v>1.6806722689075598E-2</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -955,14 +1101,17 @@
       <c r="F20" s="2">
         <v>1.6806722689075598E-2</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -975,14 +1124,17 @@
       <c r="F21" s="2">
         <v>1.6806722689075598E-2</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -995,14 +1147,17 @@
       <c r="F22" s="2">
         <v>1.4405762304921899E-2</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1015,14 +1170,17 @@
       <c r="F23" s="2">
         <v>1.32052821128451E-2</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1035,14 +1193,17 @@
       <c r="F24" s="2">
         <v>1.2004801920768301E-2</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1055,14 +1216,17 @@
       <c r="F25" s="2">
         <v>1.2004801920768301E-2</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1075,14 +1239,17 @@
       <c r="F26" s="2">
         <v>1.0804321728691399E-2</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1095,14 +1262,17 @@
       <c r="F27" s="2">
         <v>1.0804321728691399E-2</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1115,14 +1285,17 @@
       <c r="F28" s="2">
         <v>9.60384153661464E-3</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="7">
         <v>7</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1135,14 +1308,17 @@
       <c r="F29" s="2">
         <v>8.4033613445378096E-3</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1155,14 +1331,17 @@
       <c r="F30" s="2">
         <v>7.20288115246098E-3</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1175,14 +1354,17 @@
       <c r="F31" s="2">
         <v>6.0024009603841504E-3</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1193,12 +1375,15 @@
       <c r="F32" s="2">
         <v>4.80192076830732E-3</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="7"/>
+      <c r="J32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1211,14 +1396,17 @@
       <c r="F33" s="2">
         <v>3.60144057623049E-3</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1231,14 +1419,17 @@
       <c r="F34" s="2">
         <v>2.40096038415366E-3</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1251,19 +1442,17 @@
       <c r="F35" s="2">
         <v>1.20048019207683E-3</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>33</v>
+      <c r="J35" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B35" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B35">
-      <sortCondition descending="1" ref="B2:B35"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:F35">
     <sortCondition descending="1" ref="F3:F35"/>
   </sortState>
@@ -1272,6 +1461,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>